<commit_message>
Bulk Upload Funtionality merged
</commit_message>
<xml_diff>
--- a/public/admin/bulk-upload-sample.xlsx
+++ b/public/admin/bulk-upload-sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Communities" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Elevation Types" sheetId="4" r:id="rId4"/>
     <sheet name="Elevation Color Schemes" sheetId="5" r:id="rId5"/>
     <sheet name="Elevation Type Color Schemes" sheetId="6" r:id="rId6"/>
+    <sheet name="Color Scheme Features" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
   <si>
     <t>Contact Person</t>
   </si>
@@ -218,6 +219,54 @@
   </si>
   <si>
     <t>elante-mini-color-scheme-2.png</t>
+  </si>
+  <si>
+    <t>Feature Title</t>
+  </si>
+  <si>
+    <t>Feature Price</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Feature Image</t>
+  </si>
+  <si>
+    <t>Manufacturer Id</t>
+  </si>
+  <si>
+    <t>(Upgrade=1, Base=0)</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>Upgraded Type(Concrete=1, Window=2, Wall=3), Base=0</t>
+  </si>
+  <si>
+    <t>windows</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>elante-elante-basic-windows.png</t>
+  </si>
+  <si>
+    <t>Elevation or Elevation Type Title</t>
   </si>
 </sst>
 </file>
@@ -270,10 +319,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -922,7 +972,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1042,4 +1092,103 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2">
+        <v>500</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Features Import Bulk Import Added
</commit_message>
<xml_diff>
--- a/public/admin/bulk-upload-sample.xlsx
+++ b/public/admin/bulk-upload-sample.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Communities" sheetId="1" r:id="rId1"/>
     <sheet name="Elevations" sheetId="2" r:id="rId2"/>
     <sheet name="Floors" sheetId="3" r:id="rId3"/>
-    <sheet name="Elevation Types" sheetId="4" r:id="rId4"/>
-    <sheet name="Elevation Color Schemes" sheetId="5" r:id="rId5"/>
-    <sheet name="Elevation Type Color Schemes" sheetId="6" r:id="rId6"/>
-    <sheet name="Color Scheme Features" sheetId="7" r:id="rId7"/>
+    <sheet name="Floor Features" sheetId="9" r:id="rId4"/>
+    <sheet name="Elevation Types" sheetId="4" r:id="rId5"/>
+    <sheet name="Elevation Color Schemes" sheetId="5" r:id="rId6"/>
+    <sheet name="Elevation Type Color Schemes" sheetId="6" r:id="rId7"/>
+    <sheet name="Color Scheme Features" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
   <si>
     <t>Contact Person</t>
   </si>
@@ -267,6 +268,21 @@
   </si>
   <si>
     <t>Elevation or Elevation Type Title</t>
+  </si>
+  <si>
+    <t>gourment(100)</t>
+  </si>
+  <si>
+    <t>gourment(10007)</t>
+  </si>
+  <si>
+    <t>KITCHEN</t>
+  </si>
+  <si>
+    <t>(feature_group=1, feature=2)</t>
+  </si>
+  <si>
+    <t>GARAGE</t>
   </si>
 </sst>
 </file>
@@ -737,7 +753,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,7 +841,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -875,6 +891,108 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -967,7 +1085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1031,7 +1149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1094,11 +1212,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updations in Mega Import
</commit_message>
<xml_diff>
--- a/public/admin/bulk-upload-sample.xlsx
+++ b/public/admin/bulk-upload-sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Communities" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="87">
   <si>
     <t>Contact Person</t>
   </si>
@@ -283,6 +283,15 @@
   </si>
   <si>
     <t>GARAGE</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>elante-basement-gourment-100.png</t>
+  </si>
+  <si>
+    <t>elante-basement-gourment-10007.png</t>
   </si>
 </sst>
 </file>
@@ -623,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -638,9 +647,9 @@
     <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" customWidth="1"/>
-    <col min="11" max="11" width="25.5546875" customWidth="1"/>
-    <col min="12" max="12" width="30" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="63.33203125" bestFit="1" customWidth="1"/>
@@ -892,10 +901,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -905,9 +914,10 @@
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -923,8 +933,11 @@
       <c r="E1" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -938,7 +951,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -954,8 +967,11 @@
       <c r="E3">
         <v>4000</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -971,8 +987,11 @@
       <c r="E4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>41</v>
       </c>

</xml_diff>